<commit_message>
Update ims docs: 'src/generate_docs.py ims docs/ims'
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -556,7 +556,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>version</t>
   </si>
@@ -601,6 +601,12 @@
   </si>
   <si>
     <t>MALDI-IMS</t>
+  </si>
+  <si>
+    <t>MALDI-IMS-pos</t>
+  </si>
+  <si>
+    <t>MALDI-IMS-neg</t>
   </si>
   <si>
     <t>SIMS-IMS</t>
@@ -1179,88 +1185,88 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1271,8 +1277,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: MALDI-IMS / SIMS-IMS / NanoDESI / DESI." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from analyte_class list." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$6</formula1>
@@ -1348,12 +1354,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1371,12 +1377,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1394,17 +1400,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1422,7 +1428,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1474,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1492,6 +1498,16 @@
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1509,32 +1525,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1552,42 +1568,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1605,12 +1621,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1628,27 +1644,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1666,17 +1682,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mccalluc/update ims in place (#1049)
* update schema

* regen
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -248,7 +248,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The ion source type used for surface sampling (MALDI, MALDI-2, DESI, or SIMS) or LC-MS/MS data acquisition (nESI)</t>
+          <t>The ion source type used for surface sampling (MALDI, MALDI-2, DESI, nanoDESI or SIMS).</t>
         </r>
       </text>
     </comment>
@@ -556,7 +556,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>version</t>
   </si>
@@ -661,9 +661,6 @@
   </si>
   <si>
     <t>SIMS-H2O</t>
-  </si>
-  <si>
-    <t>ESI</t>
   </si>
   <si>
     <t>nanoDESI</t>
@@ -1197,73 +1194,73 @@
         <v>28</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AG1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="AJ1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1281,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from ms_source list." sqref="Q2:Q1048576">
-      <formula1>'ms_source list'!$A$1:$A$8</formula1>
+      <formula1>'ms_source list'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: negative ion mode / positive ion mode / negative and positive ion mode." sqref="R2:R1048576">
       <formula1>'polarity list'!$A$1:$A$3</formula1>
@@ -1351,12 +1348,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1374,12 +1371,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1397,17 +1394,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1425,7 +1422,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1544,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1586,11 +1583,6 @@
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1608,17 +1600,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1636,27 +1628,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1674,17 +1666,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated docs for IMS
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -18,8 +18,7 @@
     <sheet name="ms_scan_mode list" sheetId="9" r:id="rId9"/>
     <sheet name="resolution_x_unit list" sheetId="10" r:id="rId10"/>
     <sheet name="resolution_y_unit list" sheetId="11" r:id="rId11"/>
-    <sheet name="preparation_maldi_matrix list" sheetId="12" r:id="rId12"/>
-    <sheet name="desi_solvent_f...rate_unit list" sheetId="13" r:id="rId13"/>
+    <sheet name="desi_solvent_f...rate_unit list" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -556,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>version</t>
   </si>
@@ -748,15 +747,6 @@
   </si>
   <si>
     <t>preparation_maldi_matrix</t>
-  </si>
-  <si>
-    <t>CHB</t>
-  </si>
-  <si>
-    <t>DHB</t>
-  </si>
-  <si>
-    <t>SA</t>
   </si>
   <si>
     <t>desi_solvent</t>
@@ -1239,32 +1229,32 @@
         <v>63</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>75</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="20">
+  <dataValidations count="19">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1321,9 +1311,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="AB2:AB1048576">
       <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: CHB / DHB / SA." sqref="AF2:AF1048576">
-      <formula1>'preparation_maldi_matrix list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
       <formula1>-1e+307</formula1>
@@ -1386,34 +1373,6 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1422,7 +1381,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change field type of `preparation_maldi_matrix` to a string rather than restrictive enum (#1161)
* Change field type of `preparation_maldi_matrix` to a string rather than a restrictive enum that is not comprehensive of all MALDI matrices

* updated docs for IMS

* update CHANGELOG.md
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -18,8 +18,7 @@
     <sheet name="ms_scan_mode list" sheetId="9" r:id="rId9"/>
     <sheet name="resolution_x_unit list" sheetId="10" r:id="rId10"/>
     <sheet name="resolution_y_unit list" sheetId="11" r:id="rId11"/>
-    <sheet name="preparation_maldi_matrix list" sheetId="12" r:id="rId12"/>
-    <sheet name="desi_solvent_f...rate_unit list" sheetId="13" r:id="rId13"/>
+    <sheet name="desi_solvent_f...rate_unit list" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -556,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>version</t>
   </si>
@@ -748,15 +747,6 @@
   </si>
   <si>
     <t>preparation_maldi_matrix</t>
-  </si>
-  <si>
-    <t>CHB</t>
-  </si>
-  <si>
-    <t>DHB</t>
-  </si>
-  <si>
-    <t>SA</t>
   </si>
   <si>
     <t>desi_solvent</t>
@@ -1239,32 +1229,32 @@
         <v>63</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>75</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="20">
+  <dataValidations count="19">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1321,9 +1311,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="AB2:AB1048576">
       <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: CHB / DHB / SA." sqref="AF2:AF1048576">
-      <formula1>'preparation_maldi_matrix list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
       <formula1>-1e+307</formula1>
@@ -1386,34 +1373,6 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1422,7 +1381,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding DESI as an acceptable enumeration for ims-v2 ms_source element
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>version</t>
   </si>
@@ -1271,7 +1271,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from ms_source list." sqref="Q2:Q1048576">
-      <formula1>'ms_source list'!$A$1:$A$7</formula1>
+      <formula1>'ms_source list'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: negative ion mode / positive ion mode / negative and positive ion mode." sqref="R2:R1048576">
       <formula1>'polarity list'!$A$1:$A$3</formula1>
@@ -1503,7 +1503,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1541,6 +1541,11 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding DESI as an acceptable enumeration for ims-v2 ms_source element (#1178)
* Adding DESI as an acceptable enumeration for ims-v2 ms_source element

* Updated CI requirements.

---------

Co-authored-by: bhonick <bhonick-psc@pop-os.localdomain>
Co-authored-by: David Betancur <dbetancur@psc.edu>
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>version</t>
   </si>
@@ -1271,7 +1271,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from ms_source list." sqref="Q2:Q1048576">
-      <formula1>'ms_source list'!$A$1:$A$7</formula1>
+      <formula1>'ms_source list'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: negative ion mode / positive ion mode / negative and positive ion mode." sqref="R2:R1048576">
       <formula1>'polarity list'!$A$1:$A$3</formula1>
@@ -1503,7 +1503,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1541,6 +1541,11 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>